<commit_message>
Added 4 delete functions and 1 merge function
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -336,82 +336,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G2" sqref="G1:G1048576"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1">
-        <v>87</v>
-      </c>
-      <c r="J1">
-        <v>13</v>
-      </c>
-      <c r="K1">
-        <v>97</v>
+        <v>44</v>
+      </c>
+      <c r="C1">
+        <v>7</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B2">
-        <v>43</v>
-      </c>
-      <c r="J2">
-        <v>90</v>
-      </c>
-      <c r="K2">
-        <v>46</v>
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>12</v>
       </c>
-      <c r="J3">
-        <v>46</v>
-      </c>
-      <c r="K3">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>19</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>31</v>
-      </c>
-      <c r="K4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>66</v>
-      </c>
-      <c r="K5">
-        <v>26</v>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HTTP requests integration with electron
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -24,6 +24,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57,8 +61,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,54 +343,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B1">
-        <v>44</v>
-      </c>
-      <c r="C1">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D1">
+        <v>21</v>
+      </c>
+      <c r="E1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>2</v>
       </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>56</v>
-      </c>
-      <c r="B2">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>8</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>67</v>
+      </c>
+      <c r="D3" s="1">
+        <v>54</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>32</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>55</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>86</v>
+      </c>
+      <c r="D4">
+        <v>75</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Frontend enhancement and Browse files integration
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -24,10 +24,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,10 +339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -356,7 +352,7 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="D1">
         <v>21</v>
@@ -367,16 +363,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B2">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -384,7 +380,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1">
         <v>54</v>
@@ -395,16 +391,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="B4">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>86</v>
-      </c>
       <c r="D4">
-        <v>75</v>
+        <v>345</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Forms + Color If
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -28,10 +28,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -57,9 +63,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -339,82 +347,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="3" max="4" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>65</v>
       </c>
       <c r="B1">
-        <v>86</v>
-      </c>
-      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2">
+        <v>69</v>
+      </c>
+      <c r="D1" s="2">
         <v>21</v>
       </c>
       <c r="E1">
         <v>6</v>
       </c>
+      <c r="G1">
+        <v>175</v>
+      </c>
+      <c r="I1">
+        <v>174</v>
+      </c>
+      <c r="P1">
+        <v>87</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>43</v>
       </c>
       <c r="B2">
-        <v>21</v>
-      </c>
-      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>51</v>
+      </c>
+      <c r="D2" s="2">
         <v>99</v>
       </c>
       <c r="E2">
         <v>17</v>
       </c>
+      <c r="G2">
+        <v>171</v>
+      </c>
+      <c r="I2">
+        <v>128</v>
+      </c>
+      <c r="P2">
+        <v>64</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>3</v>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>35</v>
-      </c>
-      <c r="D3" s="1">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2">
+        <v>27</v>
+      </c>
+      <c r="D3" s="3">
         <v>54</v>
       </c>
       <c r="E3">
         <v>9</v>
       </c>
+      <c r="G3">
+        <v>79</v>
+      </c>
+      <c r="I3">
+        <v>76</v>
+      </c>
+      <c r="P3">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>65</v>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2">
         <v>345</v>
       </c>
       <c r="E4">
         <v>80</v>
       </c>
+      <c r="G4">
+        <v>203</v>
+      </c>
+      <c r="I4">
+        <v>138</v>
+      </c>
+      <c r="P4">
+        <v>70</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>6</v>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="D5">
+        <v>86</v>
+      </c>
+      <c r="C5" s="2">
+        <v>87</v>
+      </c>
+      <c r="D5" s="2">
         <v>22</v>
       </c>
       <c r="E5">
         <v>19</v>
+      </c>
+      <c r="G5">
+        <v>34</v>
+      </c>
+      <c r="I5">
+        <v>28</v>
+      </c>
+      <c r="P5">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Color if bugs fix
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -63,13 +63,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,13 +351,13 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="3" max="4" width="10.83203125" style="2"/>
+    <col min="3" max="5" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -372,7 +373,7 @@
       <c r="D1" s="2">
         <v>21</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="2">
         <v>6</v>
       </c>
       <c r="G1">
@@ -398,7 +399,7 @@
       <c r="D2" s="2">
         <v>99</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>17</v>
       </c>
       <c r="G2">
@@ -419,12 +420,12 @@
         <v>21</v>
       </c>
       <c r="C3" s="2">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="D3" s="3">
         <v>54</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>9</v>
       </c>
       <c r="G3">
@@ -450,7 +451,7 @@
       <c r="D4" s="2">
         <v>345</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>80</v>
       </c>
       <c r="G4">
@@ -476,7 +477,7 @@
       <c r="D5" s="2">
         <v>22</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>19</v>
       </c>
       <c r="G5">

</xml_diff>

<commit_message>
Added Graph function -  Forms - Undo handling
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -43,12 +43,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,7 +75,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -71,6 +83,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -413,10 +428,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="5">
         <v>12</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>21</v>
       </c>
       <c r="C3" s="2">
@@ -425,7 +440,7 @@
       <c r="D3" s="3">
         <v>54</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="7">
         <v>9</v>
       </c>
       <c r="G3">
@@ -488,6 +503,46 @@
       </c>
       <c r="P5">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>69</v>
+      </c>
+      <c r="B6" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>51</v>
+      </c>
+      <c r="B7" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>76</v>
+      </c>
+      <c r="B8" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>87</v>
+      </c>
+      <c r="B10" s="2">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>